<commit_message>
Changes that had not been committed - left-over commit
</commit_message>
<xml_diff>
--- a/Ensemble/Ensemble Results.xlsx
+++ b/Ensemble/Ensemble Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/Predictors_tests/Ensemble/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D659C151-281A-4741-A140-198F8332E98A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ED710A-7DBB-6149-B16C-C22BDB9F9BFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="7200" windowWidth="38400" windowHeight="21600" xr2:uid="{48603932-1842-1D4E-9EFD-0DC55C537F0D}"/>
+    <workbookView xWindow="51200" yWindow="7660" windowWidth="38400" windowHeight="20180" xr2:uid="{48603932-1842-1D4E-9EFD-0DC55C537F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>This spreadsheet contains accuracy results from the Ensemble predictor. The predictor uses folds with training/query/consequents/asnwers for Datasets and Predictors exported through Ipredict framework. Queries &amp; Corresponding consequents characteristics i.e. length, remain the same as done for previous evaluations e.g. during SUBSEQ</t>
   </si>
@@ -64,13 +64,43 @@
   </si>
   <si>
     <t>All Available Predictors Pool</t>
+  </si>
+  <si>
+    <t>All Available Predictors Pool Top 4</t>
+  </si>
+  <si>
+    <t>All Available Predictors Pool Top 3</t>
+  </si>
+  <si>
+    <t>Coppied over from above to prepare for LATEX</t>
+  </si>
+  <si>
+    <t>A lossless finds and no-one else</t>
+  </si>
+  <si>
+    <t>A lossy finds and none lossless</t>
+  </si>
+  <si>
+    <t>Everybody finds</t>
+  </si>
+  <si>
+    <t>Nobody</t>
+  </si>
+  <si>
+    <t>CPT/+ finds and no SubSeq</t>
+  </si>
+  <si>
+    <t>SubSeq finds and no CPT/+</t>
+  </si>
+  <si>
+    <t>KOSARAK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,6 +143,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -135,15 +178,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7198EF00-7BFC-F140-9526-7189E08C00F5}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,272 +516,631 @@
     <col min="1" max="1" width="23.5" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
     <col min="3" max="3" width="39.5" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.5" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="3:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="K3" s="1" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="K3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="22" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>0.47335919999999998</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>0.41289749999999997</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>0.53912413000000003</v>
       </c>
+      <c r="E23" s="4">
+        <v>0.51672759999999995</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.53460770000000002</v>
+      </c>
     </row>
     <row r="24" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>0.38840059999999998</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>0.46239975</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>0.55184440000000001</v>
       </c>
+      <c r="E24" s="4">
+        <v>0.52182214999999998</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.54515546999999998</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>0.27331256999999998</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>0.35031050000000002</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>0.43293883999999999</v>
       </c>
+      <c r="E25" s="4">
+        <v>0.37371460000000001</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.41366634000000002</v>
+      </c>
     </row>
     <row r="26" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>0.65878499999999995</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>0.68741540000000001</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>0.8256038</v>
       </c>
+      <c r="E26" s="4">
+        <v>0.80640500000000004</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.82280489999999995</v>
+      </c>
     </row>
     <row r="27" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>0.16188441000000001</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>0.38349613999999999</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>0.42882579999999998</v>
       </c>
+      <c r="E27" s="4">
+        <v>0.33842084</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.40140414000000002</v>
+      </c>
     </row>
     <row r="28" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>0.83719949999999999</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>0.91019530000000004</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>0.96140239999999999</v>
       </c>
+      <c r="E28" s="4">
+        <v>0.95260219999999995</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.96100222999999996</v>
+      </c>
     </row>
     <row r="29" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>0.34910216999999999</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>0.29823404999999997</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>0.38052097000000001</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.36977747</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.37788295999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.47335919999999998</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.41289749999999997</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.53460770000000002</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.16188441000000001</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.38349613999999999</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.40140414000000002</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.65878499999999995</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.68741540000000001</v>
+      </c>
+      <c r="D42" s="6">
+        <v>0.82280489999999995</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.34910216999999999</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.29823404999999997</v>
+      </c>
+      <c r="D43" s="6">
+        <v>0.37788295999999999</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0.83719949999999999</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.91019530000000004</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0.96100222999999996</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0.38840059999999998</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.46239975</v>
+      </c>
+      <c r="D45" s="6">
+        <v>0.54515546999999998</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0.27331256999999998</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.35031050000000002</v>
+      </c>
+      <c r="D46" s="6">
+        <v>0.41366634000000002</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="C53" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="E53" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F53" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="G53" s="8">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="C54" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="D54" s="8">
+        <v>0</v>
+      </c>
+      <c r="E54" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="F54" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="G54" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="C55" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="D55" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E55" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F55" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="G55" s="8">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="C56" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="D56" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="E56" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="F56" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G56" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="C57" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D57" s="8">
+        <v>0</v>
+      </c>
+      <c r="E57" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="F57" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="G57" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="C58" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="D58" s="8">
+        <v>0</v>
+      </c>
+      <c r="E58" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F58" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="G58" s="8">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="C59" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="D59" s="8">
+        <v>0</v>
+      </c>
+      <c r="E59" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="F59" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="G59" s="8">
+        <v>0.18</v>
       </c>
     </row>
   </sheetData>
@@ -744,5 +1149,6 @@
     <mergeCell ref="K3:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>